<commit_message>
buildings.xlsx was adapted to linear interpolation of clusters
</commit_message>
<xml_diff>
--- a/raw_inputs/buildings.xlsx
+++ b/raw_inputs/buildings.xlsx
@@ -504,7 +504,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="4">
@@ -585,7 +585,7 @@
       <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="4">
@@ -614,7 +614,7 @@
       <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="4">
@@ -676,22 +676,22 @@
         <v>32</v>
       </c>
       <c r="D6" s="4">
-        <v>110.2</v>
+        <v>2254.1720857936784</v>
       </c>
       <c r="E6">
         <v>3.125</v>
       </c>
       <c r="F6" s="6">
-        <v>1.1395999999999999</v>
+        <v>0.30323662035428967</v>
       </c>
       <c r="G6" s="6">
-        <v>1.2390000000000001</v>
+        <v>0.68502384508509895</v>
       </c>
       <c r="H6" s="6">
-        <v>0.95699999999999996</v>
+        <v>0.30252178881556097</v>
       </c>
       <c r="I6" s="6">
-        <v>0.224</v>
+        <v>0.16668666724557141</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -705,22 +705,22 @@
         <v>33</v>
       </c>
       <c r="D7" s="4">
-        <v>157.5</v>
+        <v>1106.4591367359799</v>
       </c>
       <c r="E7">
         <v>3.125</v>
       </c>
       <c r="F7" s="6">
-        <v>1.0583800000000001</v>
+        <v>0.3100912728418399</v>
       </c>
       <c r="G7" s="6">
-        <v>1.0266</v>
+        <v>0.8228516446124764</v>
       </c>
       <c r="H7" s="6">
-        <v>0.4526</v>
+        <v>0.3100912728418399</v>
       </c>
       <c r="I7" s="6">
-        <v>0.19769999999999999</v>
+        <v>0.17577443919344674</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>